<commit_message>
Enhance SpendWiseCentralPage: Add processing for Parts Categories, update state management, and improve bubble chart visualization for category analysis.
</commit_message>
<xml_diff>
--- a/public/Spend Analysis.xlsx
+++ b/public/Spend Analysis.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgnglobal365-my.sharepoint.com/personal/ramjee_ayala_tadanow_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\React_Projects\studio\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{FB50A7B0-A443-4267-873C-5B4D7478C0CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAD06CFE-7B76-432F-9ED3-A3A263F18BAC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0FC36F-CC3D-42C1-8350-3ED10282DB7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="2" xr2:uid="{D583004E-4CC7-4841-B3AD-F93097197D25}"/>
+    <workbookView xWindow="57490" yWindow="10660" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{D583004E-4CC7-4841-B3AD-F93097197D25}"/>
   </bookViews>
   <sheets>
     <sheet name="Parts" sheetId="1" r:id="rId1"/>
     <sheet name="SUPPLIERS" sheetId="2" r:id="rId2"/>
     <sheet name="SUPPLIER MIX" sheetId="3" r:id="rId3"/>
+    <sheet name="Parts Categories" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="137">
   <si>
     <t>PartNumber</t>
   </si>
@@ -401,6 +402,54 @@
   </si>
   <si>
     <t>Open Road Component</t>
+  </si>
+  <si>
+    <t>CategoryName</t>
+  </si>
+  <si>
+    <t>Powertrain &amp; Engine Systems</t>
+  </si>
+  <si>
+    <t>Core Components</t>
+  </si>
+  <si>
+    <t>Chassis &amp; Suspension</t>
+  </si>
+  <si>
+    <t>Body &amp; Exterior</t>
+  </si>
+  <si>
+    <t>Electronics &amp; Controls</t>
+  </si>
+  <si>
+    <t>Performance &amp; Sport</t>
+  </si>
+  <si>
+    <t>Heavy Duty &amp; Utility</t>
+  </si>
+  <si>
+    <t>Comfort &amp; Luxury</t>
+  </si>
+  <si>
+    <t>Support Systems</t>
+  </si>
+  <si>
+    <t>Winter &amp; Arctic</t>
+  </si>
+  <si>
+    <t>Navigation &amp; Entertainment</t>
+  </si>
+  <si>
+    <t>Touring &amp; Adventure</t>
+  </si>
+  <si>
+    <t>Storage &amp; Accessories</t>
+  </si>
+  <si>
+    <t>Marine &amp; Watercraft</t>
+  </si>
+  <si>
+    <t>Specialty &amp; Off-Road</t>
   </si>
 </sst>
 </file>
@@ -1933,8 +1982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3BEFBC9-6C43-4471-AE9A-F76019158D8E}">
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2418,4 +2467,991 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C8D19E4-ED53-442D-8034-999AACBA9FEB}">
+  <dimension ref="A1:B121"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="10.20703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.3671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>456610</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>456610</v>
+      </c>
+      <c r="B3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>456611</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>456611</v>
+      </c>
+      <c r="B5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>456612</v>
+      </c>
+      <c r="B6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>456612</v>
+      </c>
+      <c r="B7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>456613</v>
+      </c>
+      <c r="B8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>456613</v>
+      </c>
+      <c r="B9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>456614</v>
+      </c>
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>456614</v>
+      </c>
+      <c r="B11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>456615</v>
+      </c>
+      <c r="B12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>456615</v>
+      </c>
+      <c r="B13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>456616</v>
+      </c>
+      <c r="B14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>456616</v>
+      </c>
+      <c r="B15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>456617</v>
+      </c>
+      <c r="B16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>456617</v>
+      </c>
+      <c r="B17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>456618</v>
+      </c>
+      <c r="B18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>456618</v>
+      </c>
+      <c r="B19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>456619</v>
+      </c>
+      <c r="B20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>456619</v>
+      </c>
+      <c r="B21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>456620</v>
+      </c>
+      <c r="B22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23">
+        <v>456620</v>
+      </c>
+      <c r="B23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24">
+        <v>456621</v>
+      </c>
+      <c r="B24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25">
+        <v>456621</v>
+      </c>
+      <c r="B25" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26">
+        <v>456622</v>
+      </c>
+      <c r="B26" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27">
+        <v>456622</v>
+      </c>
+      <c r="B27" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28">
+        <v>456623</v>
+      </c>
+      <c r="B28" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29">
+        <v>456623</v>
+      </c>
+      <c r="B29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30">
+        <v>456624</v>
+      </c>
+      <c r="B30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31">
+        <v>456624</v>
+      </c>
+      <c r="B31" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32">
+        <v>456625</v>
+      </c>
+      <c r="B32" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33">
+        <v>456625</v>
+      </c>
+      <c r="B33" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34">
+        <v>456626</v>
+      </c>
+      <c r="B34" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35">
+        <v>456626</v>
+      </c>
+      <c r="B35" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36">
+        <v>456627</v>
+      </c>
+      <c r="B36" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37">
+        <v>456627</v>
+      </c>
+      <c r="B37" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38">
+        <v>456628</v>
+      </c>
+      <c r="B38" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39">
+        <v>456628</v>
+      </c>
+      <c r="B39" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40">
+        <v>456629</v>
+      </c>
+      <c r="B40" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41">
+        <v>456629</v>
+      </c>
+      <c r="B41" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42">
+        <v>456630</v>
+      </c>
+      <c r="B42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43">
+        <v>456630</v>
+      </c>
+      <c r="B43" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44">
+        <v>456630</v>
+      </c>
+      <c r="B44" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45">
+        <v>456631</v>
+      </c>
+      <c r="B45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46">
+        <v>456631</v>
+      </c>
+      <c r="B46" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47">
+        <v>456632</v>
+      </c>
+      <c r="B47" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48">
+        <v>456632</v>
+      </c>
+      <c r="B48" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49">
+        <v>456632</v>
+      </c>
+      <c r="B49" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50">
+        <v>456633</v>
+      </c>
+      <c r="B50" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51">
+        <v>456633</v>
+      </c>
+      <c r="B51" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52">
+        <v>456634</v>
+      </c>
+      <c r="B52" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53">
+        <v>456634</v>
+      </c>
+      <c r="B53" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54">
+        <v>456635</v>
+      </c>
+      <c r="B54" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55">
+        <v>456635</v>
+      </c>
+      <c r="B55" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56">
+        <v>456636</v>
+      </c>
+      <c r="B56" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57">
+        <v>456636</v>
+      </c>
+      <c r="B57" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58">
+        <v>456637</v>
+      </c>
+      <c r="B58" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59">
+        <v>456637</v>
+      </c>
+      <c r="B59" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60">
+        <v>456637</v>
+      </c>
+      <c r="B60" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61">
+        <v>456638</v>
+      </c>
+      <c r="B61" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62">
+        <v>456638</v>
+      </c>
+      <c r="B62" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63">
+        <v>456639</v>
+      </c>
+      <c r="B63" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64">
+        <v>456639</v>
+      </c>
+      <c r="B64" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65">
+        <v>456640</v>
+      </c>
+      <c r="B65" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66">
+        <v>456640</v>
+      </c>
+      <c r="B66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67">
+        <v>456641</v>
+      </c>
+      <c r="B67" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68">
+        <v>456641</v>
+      </c>
+      <c r="B68" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69">
+        <v>456642</v>
+      </c>
+      <c r="B69" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70">
+        <v>456642</v>
+      </c>
+      <c r="B70" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71">
+        <v>456643</v>
+      </c>
+      <c r="B71" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72">
+        <v>456643</v>
+      </c>
+      <c r="B72" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73">
+        <v>456644</v>
+      </c>
+      <c r="B73" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74">
+        <v>456644</v>
+      </c>
+      <c r="B74" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75">
+        <v>456645</v>
+      </c>
+      <c r="B75" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76">
+        <v>456645</v>
+      </c>
+      <c r="B76" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77">
+        <v>456646</v>
+      </c>
+      <c r="B77" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78">
+        <v>456646</v>
+      </c>
+      <c r="B78" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79">
+        <v>456647</v>
+      </c>
+      <c r="B79" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80">
+        <v>456647</v>
+      </c>
+      <c r="B80" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81">
+        <v>456648</v>
+      </c>
+      <c r="B81" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82">
+        <v>456648</v>
+      </c>
+      <c r="B82" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83">
+        <v>456649</v>
+      </c>
+      <c r="B83" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84">
+        <v>456649</v>
+      </c>
+      <c r="B84" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85">
+        <v>456650</v>
+      </c>
+      <c r="B85" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86">
+        <v>456650</v>
+      </c>
+      <c r="B86" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A87">
+        <v>456651</v>
+      </c>
+      <c r="B87" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A88">
+        <v>456651</v>
+      </c>
+      <c r="B88" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A89">
+        <v>456651</v>
+      </c>
+      <c r="B89" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90">
+        <v>456652</v>
+      </c>
+      <c r="B90" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91">
+        <v>456652</v>
+      </c>
+      <c r="B91" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92">
+        <v>456653</v>
+      </c>
+      <c r="B92" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93">
+        <v>456653</v>
+      </c>
+      <c r="B93" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94">
+        <v>456654</v>
+      </c>
+      <c r="B94" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95">
+        <v>456654</v>
+      </c>
+      <c r="B95" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96">
+        <v>456655</v>
+      </c>
+      <c r="B96" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97">
+        <v>456655</v>
+      </c>
+      <c r="B97" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98">
+        <v>456656</v>
+      </c>
+      <c r="B98" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99">
+        <v>456656</v>
+      </c>
+      <c r="B99" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100">
+        <v>456657</v>
+      </c>
+      <c r="B100" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101">
+        <v>456657</v>
+      </c>
+      <c r="B101" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102">
+        <v>456658</v>
+      </c>
+      <c r="B102" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103">
+        <v>456658</v>
+      </c>
+      <c r="B103" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104">
+        <v>456659</v>
+      </c>
+      <c r="B104" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105">
+        <v>456659</v>
+      </c>
+      <c r="B105" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106">
+        <v>456660</v>
+      </c>
+      <c r="B106" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107">
+        <v>456660</v>
+      </c>
+      <c r="B107" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108">
+        <v>456661</v>
+      </c>
+      <c r="B108" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109">
+        <v>456661</v>
+      </c>
+      <c r="B109" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110">
+        <v>456662</v>
+      </c>
+      <c r="B110" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111">
+        <v>456662</v>
+      </c>
+      <c r="B111" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112">
+        <v>456663</v>
+      </c>
+      <c r="B112" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113">
+        <v>456663</v>
+      </c>
+      <c r="B113" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A114">
+        <v>456664</v>
+      </c>
+      <c r="B114" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A115">
+        <v>456664</v>
+      </c>
+      <c r="B115" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A116">
+        <v>456665</v>
+      </c>
+      <c r="B116" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A117">
+        <v>456665</v>
+      </c>
+      <c r="B117" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A118">
+        <v>456666</v>
+      </c>
+      <c r="B118" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A119">
+        <v>456666</v>
+      </c>
+      <c r="B119" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A120">
+        <v>456667</v>
+      </c>
+      <c r="B120" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A121">
+        <v>456667</v>
+      </c>
+      <c r="B121" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>